<commit_message>
Atualizando dicionário de dados
</commit_message>
<xml_diff>
--- a/Dicionário_de_dados.xlsx
+++ b/Dicionário_de_dados.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{040E1115-ECCA-45D4-BF1F-434188AFA2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto - Database Application\Tratamento-de-Dados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0261D6B-7FC0-4A80-B8B3-515BBC293DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dicionário de Dados - Projeto" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -133,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,32 +147,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Batang"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="GungSuh"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="GungSuh"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="GungSuh"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="GungSuh"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -190,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -200,110 +190,46 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,174 +564,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C16"/>
+  <dimension ref="A3:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="56.7109375" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" ht="20.25" customHeight="1">
+    <row r="3" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+    </row>
+    <row r="4" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A10" s="8" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A12" s="8" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A14" s="8" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>